<commit_message>
exco_watch for continuously monitor exco result
</commit_message>
<xml_diff>
--- a/sample/test/simple.xlsx
+++ b/sample/test/simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jellydonuts\playground\excel_comment_orm\sample\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2A88A9-1410-4A75-9040-73DBE515FB2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D1510D-2D98-4391-B66F-E21C44D3FC87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15000" xr2:uid="{CD521CE3-CB81-4AD2-AA9F-DD3573C62CCF}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 key: some_str
 parser: string
 --}}
-dss</t>
+</t>
         </r>
       </text>
     </comment>

</xml_diff>